<commit_message>
added cucumber parallel plugin cucumber report updated TestReporter updated removed runner classes added Login scenarios added common steps and pages for otp mode;
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testdata.xlsx
+++ b/src/test/resources/data/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9549E5-4BB7-4294-8CBE-707CF6B1BFE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6489881D-7C3B-4662-B64D-11DC0C262A9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>emailId</t>
   </si>
@@ -53,21 +53,9 @@
     <t>RegisterPHUser_TC1</t>
   </si>
   <si>
-    <t>InvalidIdentityType_TC1</t>
-  </si>
-  <si>
-    <t>InvalidIdentityType_TC2</t>
-  </si>
-  <si>
-    <t>InvalidDateOfBirth_TC2</t>
-  </si>
-  <si>
     <t>NRIC</t>
   </si>
   <si>
-    <t>G3377467U</t>
-  </si>
-  <si>
     <t>28081990</t>
   </si>
   <si>
@@ -89,7 +77,58 @@
     <t>PASSPORT</t>
   </si>
   <si>
-    <t>k9202967</t>
+    <t>AlreadyRegisteredNRIC</t>
+  </si>
+  <si>
+    <t>IncorrectDOB</t>
+  </si>
+  <si>
+    <t>S7075119D</t>
+  </si>
+  <si>
+    <t>S7978454J</t>
+  </si>
+  <si>
+    <t>13041970</t>
+  </si>
+  <si>
+    <t>18031979</t>
+  </si>
+  <si>
+    <t>3332222</t>
+  </si>
+  <si>
+    <t>09091982</t>
+  </si>
+  <si>
+    <t>13041971</t>
+  </si>
+  <si>
+    <t>S8007195G</t>
+  </si>
+  <si>
+    <t>S8007196G</t>
+  </si>
+  <si>
+    <t>LoginToUP_TC1</t>
+  </si>
+  <si>
+    <t>EmailNotRegistered</t>
+  </si>
+  <si>
+    <t>PasswordIsIncorrect</t>
+  </si>
+  <si>
+    <t>AccountNotActivated</t>
+  </si>
+  <si>
+    <t>AccountIsLockedFor30Min</t>
+  </si>
+  <si>
+    <t>mehraj999@gmail.com</t>
+  </si>
+  <si>
+    <t>sampleTest</t>
   </si>
 </sst>
 </file>
@@ -173,13 +212,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -463,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -510,80 +550,86 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -591,20 +637,24 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -626,23 +676,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BDB032-90FD-49B6-A845-DF0B1A836E36}">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A5AC5A68-97A8-4B84-B1D2-ED86D3E24102}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FFFD7EEB-E953-455A-A3BD-76FF2471FD55}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{915209EA-3161-4AAF-AAFF-9714A8412F8D}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{A5D36204-6447-4F4B-8526-3B6AF61D384A}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{7AA239F0-385C-4DDC-A8CC-E200A9E7C094}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>